<commit_message>
Created dataprovider utility for Excel file that is used in CreateJObApiTest
</commit_message>
<xml_diff>
--- a/PhoniexTestAutomationFramework/src/test/resources/testData/PhoneixTestData.xlsx
+++ b/PhoniexTestAutomationFramework/src/test/resources/testData/PhoneixTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amol\git\repository\PhoniexTestAutomationFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1455F48-CAE0-498E-BA45-9E637157BF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AE9EF7-AE9D-466C-96CB-8B85E377F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="458" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateJobTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>username</t>
   </si>
@@ -40,6 +41,141 @@
   </si>
   <si>
     <t>iamqc</t>
+  </si>
+  <si>
+    <t>mst_service_location_id</t>
+  </si>
+  <si>
+    <t>mst_platform_id</t>
+  </si>
+  <si>
+    <t>mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t>mst_oem_id</t>
+  </si>
+  <si>
+    <t>customer__first_name</t>
+  </si>
+  <si>
+    <t>customer__last_name</t>
+  </si>
+  <si>
+    <t>customer__mobile_number</t>
+  </si>
+  <si>
+    <t>customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t>customer__email_id</t>
+  </si>
+  <si>
+    <t>customer__email_id_alt</t>
+  </si>
+  <si>
+    <t>customer_address__flat_number</t>
+  </si>
+  <si>
+    <t>customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t>customer_address__street_name</t>
+  </si>
+  <si>
+    <t>customer_address__landmark</t>
+  </si>
+  <si>
+    <t>customer_address__area</t>
+  </si>
+  <si>
+    <t>customer_address__pincode</t>
+  </si>
+  <si>
+    <t>customer_address__country</t>
+  </si>
+  <si>
+    <t>customer_address__state</t>
+  </si>
+  <si>
+    <t>customer_product__dop</t>
+  </si>
+  <si>
+    <t>customer_product__serial_number</t>
+  </si>
+  <si>
+    <t>customer_product__imei1</t>
+  </si>
+  <si>
+    <t>customer_product__imei2</t>
+  </si>
+  <si>
+    <t>customer_product__popurl</t>
+  </si>
+  <si>
+    <t>customer_product__product_id</t>
+  </si>
+  <si>
+    <t>customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t>problems__id</t>
+  </si>
+  <si>
+    <t>problems__remark</t>
+  </si>
+  <si>
+    <t>Alaina</t>
+  </si>
+  <si>
+    <t>Flatley</t>
+  </si>
+  <si>
+    <t>vru@gmail.com</t>
+  </si>
+  <si>
+    <t>cr-192</t>
+  </si>
+  <si>
+    <t>lakshadeep</t>
+  </si>
+  <si>
+    <t>kunal icon road</t>
+  </si>
+  <si>
+    <t>near mall</t>
+  </si>
+  <si>
+    <t>Saudagar</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>2025-07-31T18:30:00.000Z</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Vrushali</t>
+  </si>
+  <si>
+    <t>263264368136997</t>
+  </si>
+  <si>
+    <t>563264368136997</t>
+  </si>
+  <si>
+    <t>467643256788650</t>
+  </si>
+  <si>
+    <t>467643256788655</t>
+  </si>
+  <si>
+    <t>3445554332</t>
   </si>
 </sst>
 </file>
@@ -75,8 +211,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -400,4 +537,291 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B1970F-9CA7-4045-B09D-BE8DFBE06F92}">
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="3" max="3" width="19.9296875" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" customWidth="1"/>
+    <col min="5" max="5" width="19.06640625" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" customWidth="1"/>
+    <col min="7" max="7" width="25.9296875" customWidth="1"/>
+    <col min="8" max="8" width="26.06640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.3984375" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="12" width="31" customWidth="1"/>
+    <col min="13" max="13" width="27.19921875" customWidth="1"/>
+    <col min="14" max="14" width="24.9296875" customWidth="1"/>
+    <col min="15" max="15" width="20.59765625" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" customWidth="1"/>
+    <col min="18" max="18" width="24.46484375" customWidth="1"/>
+    <col min="19" max="19" width="28" customWidth="1"/>
+    <col min="20" max="20" width="32.73046875" customWidth="1"/>
+    <col min="21" max="21" width="24.46484375" customWidth="1"/>
+    <col min="22" max="22" width="26.46484375" customWidth="1"/>
+    <col min="23" max="23" width="24.265625" customWidth="1"/>
+    <col min="24" max="24" width="26.796875" customWidth="1"/>
+    <col min="25" max="25" width="28.9296875" customWidth="1"/>
+    <col min="26" max="26" width="14.19921875" customWidth="1"/>
+    <col min="27" max="27" width="17.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2">
+        <v>411021</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2">
+        <v>3</v>
+      </c>
+      <c r="Y2">
+        <v>3</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3">
+        <v>411021</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3">
+        <v>3</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>